<commit_message>
ep we got requirements
</commit_message>
<xml_diff>
--- a/progect IK/output_test.xlsx
+++ b/progect IK/output_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ФИО</t>
   </si>
@@ -25,7 +25,13 @@
     <t>Иван Кизикин</t>
   </si>
   <si>
+    <t>Андрей Фокин</t>
+  </si>
+  <si>
     <t>2023-06-27 21:23:11</t>
+  </si>
+  <si>
+    <t>2023-07-17 12:19:35</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +408,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
camera can catch QR-code
</commit_message>
<xml_diff>
--- a/progect IK/output_test.xlsx
+++ b/progect IK/output_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>ФИО</t>
   </si>
@@ -28,10 +28,52 @@
     <t>Андрей Фокин</t>
   </si>
   <si>
+    <t xml:space="preserve">Елена  Шалаева </t>
+  </si>
+  <si>
+    <t>МАКСИМ Вихров</t>
+  </si>
+  <si>
     <t>2023-06-27 21:23:11</t>
   </si>
   <si>
     <t>2023-07-17 12:19:35</t>
+  </si>
+  <si>
+    <t>2023-07-20 11:13:08</t>
+  </si>
+  <si>
+    <t>2023-07-23 20:25:07</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:31:13</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:33:50</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:36:15</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:39:18</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:43:53</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:48:59</t>
+  </si>
+  <si>
+    <t>2023-07-24 16:56:30</t>
+  </si>
+  <si>
+    <t>2023-07-24 17:00:39</t>
+  </si>
+  <si>
+    <t>2023-07-24 17:03:29</t>
+  </si>
+  <si>
+    <t>2023-07-24 17:05:15</t>
   </si>
 </sst>
 </file>
@@ -389,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -416,7 +458,103 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>